<commit_message>
40:1 gearbox thoughts in spreadsheet
</commit_message>
<xml_diff>
--- a/docs/motor_comparisons.xlsx
+++ b/docs/motor_comparisons.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\zaphod-bot\mechanical\reference\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\zaphod-bot\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{72AB1D8C-9540-4F3A-8B2E-408DD25946EA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25740" windowHeight="15675"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25740" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -95,7 +96,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
@@ -2539,14 +2540,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>723901</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>228601</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
@@ -2575,16 +2576,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2908,11 +2909,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:R12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2922,7 +2923,7 @@
     <col min="4" max="4" width="15.85546875" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.85546875" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" customWidth="1"/>
     <col min="13" max="13" width="10.5703125" customWidth="1"/>
     <col min="14" max="14" width="16.42578125" customWidth="1"/>
     <col min="15" max="15" width="13.140625" customWidth="1"/>
@@ -2934,7 +2935,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="4">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>6</v>
@@ -3002,23 +3003,23 @@
       </c>
       <c r="B5">
         <f>A5/$B$2</f>
-        <v>2</v>
+        <v>0.25</v>
       </c>
       <c r="C5" s="3">
         <f>B5/60</f>
-        <v>3.3333333333333333E-2</v>
+        <v>4.1666666666666666E-3</v>
       </c>
       <c r="D5">
         <f>B5*60</f>
-        <v>120</v>
+        <v>15</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" ref="E5:E12" si="0">$E$2/D5</f>
-        <v>1</v>
+        <f t="shared" ref="E5:E11" si="0">$E$2/D5</f>
+        <v>8</v>
       </c>
       <c r="F5" s="3">
         <f>E5*1000</f>
-        <v>1000</v>
+        <v>8000</v>
       </c>
       <c r="J5" t="s">
         <v>9</v>
@@ -3053,24 +3054,24 @@
         <v>100</v>
       </c>
       <c r="B6">
-        <f t="shared" ref="B6:B12" si="1">A6/$B$2</f>
-        <v>20</v>
+        <f t="shared" ref="B6:B11" si="1">A6/$B$2</f>
+        <v>2.5</v>
       </c>
       <c r="C6" s="3">
-        <f t="shared" ref="C6:C12" si="2">B6/60</f>
-        <v>0.33333333333333331</v>
+        <f t="shared" ref="C6:C11" si="2">B6/60</f>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="D6">
-        <f t="shared" ref="D6:D12" si="3">B6*60</f>
-        <v>1200</v>
+        <f t="shared" ref="D6:D11" si="3">B6*60</f>
+        <v>150</v>
       </c>
       <c r="E6" s="2">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="F6" s="3">
-        <f t="shared" ref="F6:F12" si="4">E6*1000</f>
-        <v>100</v>
+        <f t="shared" ref="F6:F11" si="4">E6*1000</f>
+        <v>800</v>
       </c>
       <c r="J6" t="s">
         <v>10</v>
@@ -3107,23 +3108,23 @@
       </c>
       <c r="B7">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>12.5</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" si="2"/>
-        <v>1.6666666666666667</v>
+        <v>0.20833333333333334</v>
       </c>
       <c r="D7">
         <f t="shared" si="3"/>
-        <v>6000</v>
+        <v>750</v>
       </c>
       <c r="E7" s="2">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.16</v>
       </c>
       <c r="F7" s="3">
         <f t="shared" si="4"/>
-        <v>20</v>
+        <v>160</v>
       </c>
       <c r="J7" t="s">
         <v>15</v>
@@ -3160,23 +3161,23 @@
       </c>
       <c r="B8">
         <f t="shared" si="1"/>
-        <v>200</v>
+        <v>25</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" si="2"/>
-        <v>3.3333333333333335</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="D8">
         <f t="shared" si="3"/>
-        <v>12000</v>
+        <v>1500</v>
       </c>
       <c r="E8" s="2">
         <f t="shared" si="0"/>
-        <v>0.01</v>
+        <v>0.08</v>
       </c>
       <c r="F8" s="3">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="J8" t="s">
         <v>14</v>
@@ -3213,23 +3214,23 @@
       </c>
       <c r="B9">
         <f t="shared" si="1"/>
-        <v>400</v>
+        <v>50</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" si="2"/>
-        <v>6.666666666666667</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="D9">
         <f t="shared" si="3"/>
-        <v>24000</v>
+        <v>3000</v>
       </c>
       <c r="E9" s="2">
         <f t="shared" si="0"/>
-        <v>5.0000000000000001E-3</v>
+        <v>0.04</v>
       </c>
       <c r="F9" s="3">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -3238,74 +3239,54 @@
       </c>
       <c r="B10">
         <f t="shared" si="1"/>
-        <v>600</v>
+        <v>75</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>1.25</v>
       </c>
       <c r="D10">
         <f t="shared" si="3"/>
-        <v>36000</v>
+        <v>4500</v>
       </c>
       <c r="E10" s="2">
-        <f t="shared" si="0"/>
-        <v>3.3333333333333335E-3</v>
+        <f>$E$2/D10</f>
+        <v>2.6666666666666668E-2</v>
       </c>
       <c r="F10" s="3">
         <f t="shared" si="4"/>
-        <v>3.3333333333333335</v>
+        <v>26.666666666666668</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>4000</v>
+        <v>3250</v>
       </c>
       <c r="B11">
         <f t="shared" si="1"/>
-        <v>800</v>
+        <v>81.25</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" si="2"/>
-        <v>13.333333333333334</v>
+        <v>1.3541666666666667</v>
       </c>
       <c r="D11">
         <f t="shared" si="3"/>
-        <v>48000</v>
+        <v>4875</v>
       </c>
       <c r="E11" s="2">
         <f t="shared" si="0"/>
-        <v>2.5000000000000001E-3</v>
+        <v>2.4615384615384615E-2</v>
       </c>
       <c r="F11" s="3">
         <f t="shared" si="4"/>
-        <v>2.5</v>
+        <v>24.615384615384617</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>4000</v>
-      </c>
-      <c r="B12">
-        <f t="shared" si="1"/>
-        <v>800</v>
-      </c>
-      <c r="C12" s="3">
-        <f t="shared" si="2"/>
-        <v>13.333333333333334</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="3"/>
-        <v>48000</v>
-      </c>
-      <c r="E12" s="2">
-        <f t="shared" si="0"/>
-        <v>2.5000000000000001E-3</v>
-      </c>
-      <c r="F12" s="3">
-        <f t="shared" si="4"/>
-        <v>2.5</v>
-      </c>
+      <c r="C12" s="3"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>